<commit_message>
feat: 新增 funky denom
</commit_message>
<xml_diff>
--- a/input/FUNKY_DENOM.xlsx
+++ b/input/FUNKY_DENOM.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\chiisen\dc_denom\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\chiisen\min_bet.ts\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BD9FAC-446C-45E7-A13A-9C22FAB0D47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2034A35B-100B-495D-BDB7-09476C648AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FUNKY" sheetId="2" r:id="rId1"/>
+    <sheet name="FUNKY_DENOM" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>

</xml_diff>